<commit_message>
in progress bufg fix
</commit_message>
<xml_diff>
--- a/SampleInputFiles/sample_InProgress_argentina.xlsx
+++ b/SampleInputFiles/sample_InProgress_argentina.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vishn\OneDrive\Desktop\MyEngineering\golocalrefactor\SampleInputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7623BA5B-7897-4C17-B5CF-CF3E8DF26012}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54109710-41CC-4938-8808-8F108787C092}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4667" yWindow="0" windowWidth="24973" windowHeight="10153" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-93" windowWidth="24853" windowHeight="14586" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roadmap" sheetId="1" r:id="rId1"/>
     <sheet name="Countries" sheetId="2" r:id="rId2"/>
     <sheet name="Argentina_Specific" sheetId="3" r:id="rId3"/>
-    <sheet name="Argentina_Wrkld" sheetId="4" r:id="rId4"/>
-    <sheet name="Argentina_MCIO" sheetId="5" r:id="rId5"/>
+    <sheet name="Argentina_MCIO" sheetId="5" r:id="rId4"/>
+    <sheet name="Argentina_Wrkld" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -404,13 +404,13 @@
     </r>
   </si>
   <si>
-    <t>Johannesburg (JNB20)</t>
-  </si>
-  <si>
-    <t>Cape Town (CPT20)</t>
-  </si>
-  <si>
-    <t>Johannesburg (JNB21)</t>
+    <t>Cape Town (CPT  20)</t>
+  </si>
+  <si>
+    <t>Johannesburg (JNB  20)</t>
+  </si>
+  <si>
+    <t>Johannesburg (JNB  21)</t>
   </si>
 </sst>
 </file>
@@ -1019,6 +1019,9 @@
     <xf numFmtId="164" fontId="5" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="17" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1078,9 +1081,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1364,60 +1364,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
     <row r="1" spans="1:16" ht="20.7" x14ac:dyDescent="0.7">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="55"/>
     </row>
     <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.5">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="56" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="59" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="62" t="s">
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="63"/>
+      <c r="P2" s="64"/>
     </row>
     <row r="3" spans="1:16" ht="43" x14ac:dyDescent="0.5">
-      <c r="A3" s="55"/>
+      <c r="A3" s="56"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1586,7 +1586,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1598,7 +1598,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="65" t="s">
         <v>109</v>
       </c>
       <c r="B1" s="18" t="s">
@@ -1609,8 +1609,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A2" s="64"/>
-      <c r="B2" s="65" t="s">
+      <c r="A2" s="65"/>
+      <c r="B2" s="66" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="20" t="s">
@@ -1621,8 +1621,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A3" s="64"/>
-      <c r="B3" s="65"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="66"/>
       <c r="C3" s="21" t="s">
         <v>33</v>
       </c>
@@ -1631,8 +1631,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A4" s="64"/>
-      <c r="B4" s="65"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="21" t="s">
         <v>34</v>
       </c>
@@ -1641,8 +1641,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A5" s="64"/>
-      <c r="B5" s="65" t="s">
+      <c r="A5" s="65"/>
+      <c r="B5" s="66" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="20" t="s">
@@ -1653,8 +1653,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A6" s="64"/>
-      <c r="B6" s="65"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="21" t="s">
         <v>36</v>
       </c>
@@ -1663,18 +1663,18 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A7" s="64"/>
+      <c r="A7" s="65"/>
       <c r="B7" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="52" t="s">
         <v>111</v>
       </c>
       <c r="D7" s="24"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A8" s="64"/>
-      <c r="B8" s="66" t="s">
+      <c r="A8" s="65"/>
+      <c r="B8" s="67" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="17" t="s">
@@ -1683,32 +1683,32 @@
       <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A9" s="64"/>
-      <c r="B9" s="66"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="17" t="s">
         <v>40</v>
       </c>
       <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A10" s="64"/>
-      <c r="B10" s="66"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="17" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A11" s="64"/>
-      <c r="B11" s="66"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="17" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A12" s="64"/>
-      <c r="B12" s="66" t="s">
+      <c r="A12" s="65"/>
+      <c r="B12" s="67" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="17" t="s">
@@ -1717,8 +1717,8 @@
       <c r="D12" s="17"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A13" s="64"/>
-      <c r="B13" s="66"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="67"/>
       <c r="C13" s="25" t="s">
         <v>45</v>
       </c>
@@ -1738,6 +1738,758 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46CF6CC-FED6-4037-BDB6-B1421048F8AA}">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="24.8203125" customWidth="1"/>
+    <col min="2" max="2" width="28.5859375" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="22.5859375" customWidth="1"/>
+    <col min="5" max="5" width="29.52734375" customWidth="1"/>
+    <col min="6" max="6" width="23.76171875" customWidth="1"/>
+    <col min="7" max="7" width="39.41015625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="72" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+    </row>
+    <row r="2" spans="1:7" ht="86" x14ac:dyDescent="0.5">
+      <c r="A2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A3" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C3" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D3" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="43">
+        <v>3</v>
+      </c>
+      <c r="G3" s="44">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A4" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C4" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D4" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="43">
+        <v>3</v>
+      </c>
+      <c r="G4" s="44">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A5" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C5" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D5" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="43">
+        <v>3</v>
+      </c>
+      <c r="G5" s="44">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A6" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C6" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D6" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="43">
+        <v>3</v>
+      </c>
+      <c r="G6" s="44">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A7" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C7" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D7" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="43">
+        <v>3</v>
+      </c>
+      <c r="G7" s="45">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A8" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C8" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D8" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="43">
+        <v>3</v>
+      </c>
+      <c r="G8" s="45">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A9" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D9" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A10" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D10" s="49">
+        <v>42005</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A11" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D11" s="49">
+        <v>42005</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" s="48">
+        <v>40544</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="72"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+    </row>
+    <row r="13" spans="1:7" ht="86" x14ac:dyDescent="0.5">
+      <c r="A13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A14" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C14" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D14" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="43">
+        <v>3</v>
+      </c>
+      <c r="G14" s="44">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A15" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C15" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D15" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="43">
+        <v>3</v>
+      </c>
+      <c r="G15" s="44">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A16" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C16" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D16" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="43">
+        <v>3</v>
+      </c>
+      <c r="G16" s="44">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A17" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C17" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D17" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="43">
+        <v>3</v>
+      </c>
+      <c r="G17" s="44">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A18" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C18" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D18" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="43">
+        <v>3</v>
+      </c>
+      <c r="G18" s="45">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A19" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C19" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D19" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="43">
+        <v>3</v>
+      </c>
+      <c r="G19" s="45">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A20" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D20" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" s="48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A21" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D21" s="49">
+        <v>42005</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" s="48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A22" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D22" s="49">
+        <v>42005</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="48">
+        <v>40544</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="72" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+    </row>
+    <row r="24" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A24" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" s="40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A25" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C25" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D25" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="43">
+        <v>3</v>
+      </c>
+      <c r="G25" s="44">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A26" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C26" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D26" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E26" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F26" s="43">
+        <v>3</v>
+      </c>
+      <c r="G26" s="44">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A27" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C27" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D27" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="43">
+        <v>3</v>
+      </c>
+      <c r="G27" s="44">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A28" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B28" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C28" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D28" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E28" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="43">
+        <v>3</v>
+      </c>
+      <c r="G28" s="44">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A29" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C29" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D29" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E29" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" s="43">
+        <v>3</v>
+      </c>
+      <c r="G29" s="45">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A30" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="19">
+        <v>42370</v>
+      </c>
+      <c r="C30" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D30" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" s="43">
+        <v>3</v>
+      </c>
+      <c r="G30" s="45">
+        <v>36924</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A31" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B31" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D31" s="22">
+        <v>42006</v>
+      </c>
+      <c r="E31" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" s="48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A32" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D32" s="49">
+        <v>42005</v>
+      </c>
+      <c r="E32" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="G32" s="48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A33" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="22">
+        <v>42006</v>
+      </c>
+      <c r="D33" s="49">
+        <v>42005</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="F33" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="G33" s="48">
+        <v>40544</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A23:G23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C942CC7-50D8-4951-BAC9-A70D255278BD}">
   <dimension ref="A1:J35"/>
   <sheetViews>
@@ -1780,7 +2532,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="68" t="s">
         <v>55</v>
       </c>
       <c r="B2" s="29" t="s">
@@ -1812,7 +2564,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="68"/>
+      <c r="A3" s="69"/>
       <c r="B3" s="29" t="s">
         <v>59</v>
       </c>
@@ -1842,7 +2594,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="68"/>
+      <c r="A4" s="69"/>
       <c r="B4" s="29" t="s">
         <v>60</v>
       </c>
@@ -1872,7 +2624,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="72" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="68"/>
+      <c r="A5" s="69"/>
       <c r="B5" s="29" t="s">
         <v>61</v>
       </c>
@@ -1902,7 +2654,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="57.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="68"/>
+      <c r="A6" s="69"/>
       <c r="B6" s="29" t="s">
         <v>63</v>
       </c>
@@ -1932,7 +2684,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="68"/>
+      <c r="A7" s="69"/>
       <c r="B7" s="29" t="s">
         <v>65</v>
       </c>
@@ -1962,7 +2714,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="68"/>
+      <c r="A8" s="69"/>
       <c r="B8" s="29" t="s">
         <v>67</v>
       </c>
@@ -1992,7 +2744,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="69"/>
+      <c r="A9" s="70"/>
       <c r="B9" s="35" t="s">
         <v>17</v>
       </c>
@@ -2022,7 +2774,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="68" t="s">
         <v>70</v>
       </c>
       <c r="B10" s="29" t="s">
@@ -2054,7 +2806,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="68"/>
+      <c r="A11" s="69"/>
       <c r="B11" s="29" t="s">
         <v>71</v>
       </c>
@@ -2084,7 +2836,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="68"/>
+      <c r="A12" s="69"/>
       <c r="B12" s="29" t="s">
         <v>73</v>
       </c>
@@ -2114,7 +2866,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="72" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="68"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="29" t="s">
         <v>61</v>
       </c>
@@ -2144,7 +2896,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="57.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="68"/>
+      <c r="A14" s="69"/>
       <c r="B14" s="29" t="s">
         <v>63</v>
       </c>
@@ -2174,7 +2926,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="29" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="68"/>
+      <c r="A15" s="69"/>
       <c r="B15" s="29" t="s">
         <v>65</v>
       </c>
@@ -2204,7 +2956,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="68"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="29" t="s">
         <v>67</v>
       </c>
@@ -2234,7 +2986,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="69"/>
+      <c r="A17" s="70"/>
       <c r="B17" s="35" t="s">
         <v>17</v>
       </c>
@@ -2264,7 +3016,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="67" t="s">
+      <c r="A18" s="68" t="s">
         <v>76</v>
       </c>
       <c r="B18" s="29" t="s">
@@ -2296,7 +3048,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="68"/>
+      <c r="A19" s="69"/>
       <c r="B19" s="29" t="s">
         <v>77</v>
       </c>
@@ -2326,7 +3078,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="68"/>
+      <c r="A20" s="69"/>
       <c r="B20" s="29" t="s">
         <v>73</v>
       </c>
@@ -2356,7 +3108,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="72" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="68"/>
+      <c r="A21" s="69"/>
       <c r="B21" s="29" t="s">
         <v>61</v>
       </c>
@@ -2386,7 +3138,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="57.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="68"/>
+      <c r="A22" s="69"/>
       <c r="B22" s="29" t="s">
         <v>63</v>
       </c>
@@ -2416,7 +3168,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="68"/>
+      <c r="A23" s="69"/>
       <c r="B23" s="29" t="s">
         <v>65</v>
       </c>
@@ -2446,7 +3198,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="68"/>
+      <c r="A24" s="69"/>
       <c r="B24" s="29" t="s">
         <v>67</v>
       </c>
@@ -2476,7 +3228,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="69"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="35" t="s">
         <v>17</v>
       </c>
@@ -2506,7 +3258,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="67" t="s">
+      <c r="A26" s="68" t="s">
         <v>82</v>
       </c>
       <c r="B26" s="29" t="s">
@@ -2538,7 +3290,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="72" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="68"/>
+      <c r="A27" s="69"/>
       <c r="B27" s="29" t="s">
         <v>61</v>
       </c>
@@ -2568,7 +3320,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="57.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="68"/>
+      <c r="A28" s="69"/>
       <c r="B28" s="29" t="s">
         <v>63</v>
       </c>
@@ -2598,7 +3350,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="68"/>
+      <c r="A29" s="69"/>
       <c r="B29" s="29" t="s">
         <v>65</v>
       </c>
@@ -2628,7 +3380,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="70"/>
+      <c r="A30" s="71"/>
       <c r="B30" s="38" t="s">
         <v>17</v>
       </c>
@@ -2658,7 +3410,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="67" t="s">
+      <c r="A31" s="68" t="s">
         <v>89</v>
       </c>
       <c r="B31" s="29" t="s">
@@ -2690,7 +3442,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="72" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="68"/>
+      <c r="A32" s="69"/>
       <c r="B32" s="29" t="s">
         <v>61</v>
       </c>
@@ -2720,7 +3472,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" ht="57.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="68"/>
+      <c r="A33" s="69"/>
       <c r="B33" s="29" t="s">
         <v>63</v>
       </c>
@@ -2750,7 +3502,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="68"/>
+      <c r="A34" s="69"/>
       <c r="B34" s="29" t="s">
         <v>65</v>
       </c>
@@ -2780,7 +3532,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" ht="43.35" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="70"/>
+      <c r="A35" s="71"/>
       <c r="B35" s="38" t="s">
         <v>17</v>
       </c>
@@ -2819,755 +3571,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46CF6CC-FED6-4037-BDB6-B1421048F8AA}">
-  <dimension ref="A1:G33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:G23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="2" max="2" width="28.5859375" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="22.5859375" customWidth="1"/>
-    <col min="5" max="5" width="39.9375" customWidth="1"/>
-    <col min="6" max="6" width="51.52734375" customWidth="1"/>
-    <col min="7" max="7" width="93.703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="71" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-    </row>
-    <row r="2" spans="1:7" ht="86" x14ac:dyDescent="0.5">
-      <c r="A2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" s="40" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A3" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C3" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D3" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="43">
-        <v>3</v>
-      </c>
-      <c r="G3" s="44">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A4" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C4" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D4" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E4" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="43">
-        <v>3</v>
-      </c>
-      <c r="G4" s="44">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A5" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C5" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D5" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="43">
-        <v>3</v>
-      </c>
-      <c r="G5" s="44">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A6" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C6" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D6" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" s="43">
-        <v>3</v>
-      </c>
-      <c r="G6" s="44">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A7" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C7" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D7" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" s="43">
-        <v>3</v>
-      </c>
-      <c r="G7" s="45">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A8" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C8" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D8" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F8" s="43">
-        <v>3</v>
-      </c>
-      <c r="G8" s="45">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A9" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D9" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F9" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="G9" s="48" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A10" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D10" s="49">
-        <v>42005</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F10" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="G10" s="48" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A11" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D11" s="49">
-        <v>42005</v>
-      </c>
-      <c r="E11" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" s="48">
-        <v>40544</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="71" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-    </row>
-    <row r="13" spans="1:7" ht="86" x14ac:dyDescent="0.5">
-      <c r="A13" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="G13" s="40" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A14" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C14" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D14" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E14" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F14" s="43">
-        <v>3</v>
-      </c>
-      <c r="G14" s="44">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A15" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C15" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D15" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E15" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F15" s="43">
-        <v>3</v>
-      </c>
-      <c r="G15" s="44">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A16" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C16" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D16" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E16" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F16" s="43">
-        <v>3</v>
-      </c>
-      <c r="G16" s="44">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A17" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="B17" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C17" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D17" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E17" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F17" s="43">
-        <v>3</v>
-      </c>
-      <c r="G17" s="44">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A18" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="B18" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C18" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D18" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F18" s="43">
-        <v>3</v>
-      </c>
-      <c r="G18" s="45">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A19" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="B19" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C19" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D19" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F19" s="43">
-        <v>3</v>
-      </c>
-      <c r="G19" s="45">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A20" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="B20" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D20" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F20" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="G20" s="48" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A21" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D21" s="49">
-        <v>42005</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="48" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A22" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D22" s="49">
-        <v>42005</v>
-      </c>
-      <c r="E22" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" s="48">
-        <v>40544</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="71" t="s">
-        <v>114</v>
-      </c>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-    </row>
-    <row r="24" spans="1:7" ht="86" x14ac:dyDescent="0.5">
-      <c r="A24" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B24" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24" s="40" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A25" s="41" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C25" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D25" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E25" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" s="43">
-        <v>3</v>
-      </c>
-      <c r="G25" s="44">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A26" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C26" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D26" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E26" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F26" s="43">
-        <v>3</v>
-      </c>
-      <c r="G26" s="44">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A27" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C27" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D27" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E27" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F27" s="43">
-        <v>3</v>
-      </c>
-      <c r="G27" s="44">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A28" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C28" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D28" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E28" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" s="43">
-        <v>3</v>
-      </c>
-      <c r="G28" s="44">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A29" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C29" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D29" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E29" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F29" s="43">
-        <v>3</v>
-      </c>
-      <c r="G29" s="45">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A30" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="19">
-        <v>42370</v>
-      </c>
-      <c r="C30" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D30" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E30" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" s="43">
-        <v>3</v>
-      </c>
-      <c r="G30" s="45">
-        <v>36924</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A31" s="41" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D31" s="22">
-        <v>42006</v>
-      </c>
-      <c r="E31" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F31" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="G31" s="48" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A32" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D32" s="49">
-        <v>42005</v>
-      </c>
-      <c r="E32" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F32" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="G32" s="48" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A33" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="22">
-        <v>42006</v>
-      </c>
-      <c r="D33" s="49">
-        <v>42005</v>
-      </c>
-      <c r="E33" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="F33" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="G33" s="48">
-        <v>40544</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A23:G23"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>